<commit_message>
Mise a jour du Wireframe
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Remplissage du journal de travail avec les heures que j'ai noté sur papier.</t>
+  </si>
+  <si>
+    <t>Modification des maquettes du site.</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
   <dimension ref="A1:N1099"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,16 +735,26 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="5"/>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>44966</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.61041666666666672</v>
+      </c>
       <c r="D7" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+        <v>4.7916666666666718E-2</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout du diagramme de flux
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Modification des maquettes du site.</t>
+  </si>
+  <si>
+    <t>Création du diagramme de flux.</t>
   </si>
 </sst>
 </file>
@@ -590,7 +593,7 @@
   <dimension ref="A1:N1099"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,15 +761,25 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="7">
+        <v>44966</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="D8" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+        <v>5.902777777777779E-2</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modification du Wireframe et ajout du Use case
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Maquettes</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>Continuation du diagramme de flux.</t>
+  </si>
+  <si>
+    <t>Continuation des maquettes du site.</t>
+  </si>
+  <si>
+    <t>Création du use case.</t>
   </si>
 </sst>
 </file>
@@ -596,7 +599,7 @@
   <dimension ref="A1:N1099"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,10 +649,10 @@
         <v>2.0833333333333925E-2</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="18"/>
     </row>
@@ -671,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -690,10 +693,10 @@
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="11"/>
     </row>
@@ -712,10 +715,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="15"/>
     </row>
@@ -734,10 +737,10 @@
         <v>3.125E-2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -756,10 +759,10 @@
         <v>4.7916666666666718E-2</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="12"/>
     </row>
@@ -778,10 +781,10 @@
         <v>5.902777777777779E-2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="11"/>
     </row>
@@ -800,10 +803,10 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
@@ -829,10 +832,10 @@
         <v>7.6388888888888618E-3</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
@@ -843,53 +846,93 @@
       <c r="M10" s="6"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>44979</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.62152777777777779</v>
+      </c>
       <c r="D11" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>44979</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.64374999999999993</v>
+      </c>
       <c r="D12" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+        <v>2.1527777777777701E-2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="G12" s="11"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>44979</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.64722222222222225</v>
+      </c>
       <c r="D13" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+        <v>2.7777777777777679E-3</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="G13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="7">
+        <v>44979</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.66875000000000007</v>
+      </c>
       <c r="D14" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout des PDF du Use case et du Wireframe
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -921,11 +921,11 @@
         <v>0.6479166666666667</v>
       </c>
       <c r="C14" s="8">
-        <v>0.66875000000000007</v>
+        <v>0.6743055555555556</v>
       </c>
       <c r="D14" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>2.6388888888888906E-2</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Ajout de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Création du use case.</t>
+  </si>
+  <si>
+    <t>Création de la documentation du projet.</t>
   </si>
 </sst>
 </file>
@@ -599,7 +602,7 @@
   <dimension ref="A1:N1099"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,16 +938,26 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>44979</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.67499999999999993</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D15" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+        <v>2.9861111111111227E-2</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update of the Documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Création du footer avec Romain.</t>
+  </si>
+  <si>
+    <t>Prise de connaissance du code complet de Romain pour la suite avec son aide.</t>
+  </si>
+  <si>
+    <t>Ajout des analyses de sprints sur la doc et ajout des répértoires pour le dossier de réalisation physique.</t>
+  </si>
+  <si>
+    <t>Création de la page de basket.</t>
+  </si>
+  <si>
+    <t>Ajout de tous les schemas et des logiciels utilisé et leur version dans la documentation.</t>
   </si>
 </sst>
 </file>
@@ -628,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1099"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K22" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,52 +1227,94 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>44993</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D26" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+        <v>2.5694444444444464E-2</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>44994</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.60069444444444442</v>
+      </c>
       <c r="D27" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
+      <c r="A28" s="7">
+        <v>44999</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C28" s="8">
+        <v>0.70624999999999993</v>
+      </c>
       <c r="D28" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+        <v>3.2638888888888773E-2</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="G28" s="18"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>45000</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="D29" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update of the documentation 2
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
+++ b/Documentation/Journal_de_travail/Sacha Jaccard/Journal de travail Sacha.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Ajout de tous les schemas et des logiciels utilisé et leur version dans la documentation.</t>
+  </si>
+  <si>
+    <t>Ajout dans la documentation des ajout de Romain suite à un problème technique.</t>
   </si>
 </sst>
 </file>
@@ -640,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1099"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K22" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,16 +1320,24 @@
       </c>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>45006</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0.67013888888888884</v>
+      </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+        <v>-0.67013888888888884</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>